<commit_message>
£SHOE FY20/1 results, valuation metrics
</commit_message>
<xml_diff>
--- a/£SHOE.xlsx
+++ b/£SHOE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCE5402-83AE-A848-8907-178874BD0C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8C9D5D-1499-4D4E-A4E2-55172DDE2247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="18900" activeTab="1" xr2:uid="{C965C64C-6189-49A9-ABBD-37EA87F8BC3F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="119">
   <si>
     <t>£SHOE</t>
   </si>
@@ -387,17 +387,25 @@
   </si>
   <si>
     <t>Energy prices are fixed until September 2023, which should offset any market volatility from Ukraine war</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(Projected)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,8 +478,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +515,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -596,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -715,6 +743,47 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="9" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -811,8 +880,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -827,8 +896,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7734300" y="9525"/>
-          <a:ext cx="0" cy="11553825"/>
+          <a:off x="8858250" y="9525"/>
+          <a:ext cx="0" cy="17478375"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -861,8 +930,8 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -877,8 +946,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13230225" y="0"/>
-          <a:ext cx="0" cy="11553825"/>
+          <a:off x="15154275" y="0"/>
+          <a:ext cx="0" cy="18669000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1204,7 +1273,7 @@
   <dimension ref="A2:Q39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1266,10 +1335,14 @@
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1">
-        <v>48.5</v>
-      </c>
-      <c r="D7" s="18"/>
+      <c r="C7" s="53">
+        <f>'Financial Model'!K18</f>
+        <v>50</v>
+      </c>
+      <c r="D7" s="18" t="str">
+        <f>$C$29</f>
+        <v>H122</v>
+      </c>
       <c r="G7" s="16"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
@@ -1288,7 +1361,7 @@
       </c>
       <c r="C8" s="5">
         <f>C6*C7</f>
-        <v>116.64249999999998</v>
+        <v>120.24999999999999</v>
       </c>
       <c r="D8" s="18"/>
       <c r="G8" s="16"/>
@@ -1385,7 +1458,7 @@
       </c>
       <c r="C12" s="6">
         <f>C8-C11</f>
-        <v>102.77049999999998</v>
+        <v>106.37799999999999</v>
       </c>
       <c r="D12" s="19"/>
       <c r="G12" s="16"/>
@@ -1739,15 +1812,21 @@
       <c r="B34" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="44"/>
-      <c r="D34" s="45"/>
+      <c r="C34" s="62">
+        <f>C6/'Financial Model'!K66</f>
+        <v>4.0893015030946032</v>
+      </c>
+      <c r="D34" s="63"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="62">
+        <f>C8/SUM('Financial Model'!J6:K6)</f>
+        <v>0.80937733474231166</v>
+      </c>
+      <c r="D35" s="63"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="16" t="s">
@@ -1760,8 +1839,11 @@
       <c r="B37" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="44"/>
-      <c r="D37" s="45"/>
+      <c r="C37" s="62">
+        <f>C6/SUM('Financial Model'!J17:K17)</f>
+        <v>10.025846256461564</v>
+      </c>
+      <c r="D37" s="63"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="16" t="s">
@@ -1813,13 +1895,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126391AC-57CA-49E9-B45F-00CA8473774D}">
-  <dimension ref="B1:AE78"/>
+  <dimension ref="B1:AE85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N47" sqref="N47"/>
+      <selection activeCell="E45" sqref="E45"/>
+      <selection pane="topRight" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <selection pane="bottomRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1838,7 +1921,9 @@
     <col min="12" max="12" width="9.1640625" style="25"/>
     <col min="13" max="13" width="9.1640625" style="1"/>
     <col min="14" max="14" width="9.1640625" style="25"/>
-    <col min="15" max="16384" width="9.1640625" style="1"/>
+    <col min="15" max="20" width="9.1640625" style="1"/>
+    <col min="21" max="21" width="9.1640625" style="74"/>
+    <col min="22" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:31" s="20" customFormat="1" x14ac:dyDescent="0.15">
@@ -1890,7 +1975,7 @@
       <c r="T1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="75" t="s">
         <v>52</v>
       </c>
       <c r="V1" s="20" t="s">
@@ -1928,28 +2013,50 @@
       <c r="B2" s="21"/>
       <c r="D2" s="24"/>
       <c r="F2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="H2" s="64">
+        <f>S2</f>
+        <v>44107</v>
+      </c>
       <c r="I2" s="27">
         <v>44289</v>
       </c>
-      <c r="J2" s="24"/>
+      <c r="J2" s="64">
+        <f>T2</f>
+        <v>44471</v>
+      </c>
       <c r="K2" s="27">
         <v>44653</v>
       </c>
       <c r="L2" s="24"/>
       <c r="N2" s="24"/>
+      <c r="S2" s="27">
+        <v>44107</v>
+      </c>
+      <c r="T2" s="27">
+        <v>44471</v>
+      </c>
+      <c r="U2" s="76" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="3" spans="2:31" s="22" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="21"/>
       <c r="D3" s="24"/>
       <c r="F3" s="24"/>
       <c r="H3" s="24"/>
-      <c r="J3" s="24"/>
+      <c r="J3" s="66">
+        <f>T3</f>
+        <v>11324</v>
+      </c>
       <c r="K3" s="28">
         <v>45063</v>
       </c>
       <c r="L3" s="24"/>
       <c r="N3" s="24"/>
+      <c r="T3" s="65">
+        <v>11324</v>
+      </c>
+      <c r="U3" s="76"/>
     </row>
     <row r="4" spans="2:31" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B4" s="39" t="s">
@@ -1957,16 +2064,26 @@
       </c>
       <c r="D4" s="40"/>
       <c r="F4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="H4" s="67"/>
       <c r="I4" s="39">
         <v>22.8</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="67">
+        <f>T4-I4</f>
+        <v>65.8</v>
+      </c>
       <c r="K4" s="39">
         <v>58.1</v>
       </c>
       <c r="L4" s="40"/>
       <c r="N4" s="40"/>
+      <c r="S4" s="39">
+        <v>103</v>
+      </c>
+      <c r="T4" s="39">
+        <v>88.6</v>
+      </c>
+      <c r="U4" s="73"/>
     </row>
     <row r="5" spans="2:31" s="39" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="39" t="s">
@@ -1974,16 +2091,26 @@
       </c>
       <c r="D5" s="40"/>
       <c r="F5" s="40"/>
-      <c r="H5" s="40"/>
+      <c r="H5" s="67"/>
       <c r="I5" s="39">
         <v>17.600000000000001</v>
       </c>
-      <c r="J5" s="40"/>
+      <c r="J5" s="67">
+        <f>T5-I5</f>
+        <v>12.899999999999999</v>
+      </c>
       <c r="K5" s="39">
         <v>11.8</v>
       </c>
       <c r="L5" s="40"/>
       <c r="N5" s="40"/>
+      <c r="S5" s="39">
+        <v>19.3</v>
+      </c>
+      <c r="T5" s="39">
+        <v>30.5</v>
+      </c>
+      <c r="U5" s="73"/>
     </row>
     <row r="6" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2" t="s">
@@ -1995,22 +2122,49 @@
       <c r="I6" s="31">
         <v>40.435000000000002</v>
       </c>
-      <c r="J6" s="30"/>
+      <c r="J6" s="69">
+        <f>T6-I6</f>
+        <v>78.706999999999994</v>
+      </c>
       <c r="K6" s="31">
         <v>69.864000000000004</v>
       </c>
-      <c r="L6" s="30"/>
+      <c r="L6" s="72">
+        <f>U6-K6</f>
+        <v>63.575040000000001</v>
+      </c>
       <c r="N6" s="30"/>
+      <c r="S6" s="31">
+        <v>122.568</v>
+      </c>
+      <c r="T6" s="31">
+        <v>119.142</v>
+      </c>
+      <c r="U6" s="77">
+        <f>T6*(1+U21)</f>
+        <v>133.43904000000001</v>
+      </c>
     </row>
     <row r="7" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C7" s="53"/>
       <c r="I7" s="5">
         <v>32.688000000000002</v>
       </c>
+      <c r="J7" s="67">
+        <f>T7-I7</f>
+        <v>53.978999999999999</v>
+      </c>
       <c r="K7" s="5">
         <v>56.247</v>
+      </c>
+      <c r="S7" s="5">
+        <v>117.33199999999999</v>
+      </c>
+      <c r="T7" s="5">
+        <v>86.667000000000002</v>
       </c>
     </row>
     <row r="8" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -2024,13 +2178,25 @@
         <f>I6-I7</f>
         <v>7.7469999999999999</v>
       </c>
-      <c r="J8" s="30"/>
+      <c r="J8" s="69">
+        <f>J6-J7</f>
+        <v>24.727999999999994</v>
+      </c>
       <c r="K8" s="31">
         <f>K6-K7</f>
         <v>13.617000000000004</v>
       </c>
       <c r="L8" s="30"/>
       <c r="N8" s="30"/>
+      <c r="S8" s="31">
+        <f t="shared" ref="S8" si="0">S6-S7</f>
+        <v>5.2360000000000042</v>
+      </c>
+      <c r="T8" s="31">
+        <f>T6-T7</f>
+        <v>32.474999999999994</v>
+      </c>
+      <c r="U8" s="78"/>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
@@ -2039,8 +2205,18 @@
       <c r="I9" s="5">
         <v>7.9059999999999997</v>
       </c>
+      <c r="J9" s="67">
+        <f t="shared" ref="J9:J10" si="1">T9-I9</f>
+        <v>9.0560000000000009</v>
+      </c>
       <c r="K9" s="5">
         <v>7.508</v>
+      </c>
+      <c r="S9" s="5">
+        <v>13.928000000000001</v>
+      </c>
+      <c r="T9" s="5">
+        <v>16.962</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.15">
@@ -2050,8 +2226,18 @@
       <c r="I10" s="5">
         <v>1.593</v>
       </c>
+      <c r="J10" s="67">
+        <f t="shared" si="1"/>
+        <v>2.9059999999999997</v>
+      </c>
       <c r="K10" s="5">
         <v>2.448</v>
+      </c>
+      <c r="S10" s="5">
+        <v>4.0179999999999998</v>
+      </c>
+      <c r="T10" s="5">
+        <v>4.4989999999999997</v>
       </c>
     </row>
     <row r="11" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -2065,13 +2251,25 @@
         <f>+I8-I9-I10</f>
         <v>-1.7519999999999998</v>
       </c>
-      <c r="J11" s="30"/>
+      <c r="J11" s="69">
+        <f>+J8-J9-J10</f>
+        <v>12.765999999999995</v>
+      </c>
       <c r="K11" s="31">
         <f>+K8-K9-K10</f>
         <v>3.6610000000000045</v>
       </c>
       <c r="L11" s="30"/>
       <c r="N11" s="30"/>
+      <c r="S11" s="31">
+        <f t="shared" ref="S11:T11" si="2">+S8-S9-S10</f>
+        <v>-12.709999999999997</v>
+      </c>
+      <c r="T11" s="31">
+        <f t="shared" si="2"/>
+        <v>11.013999999999996</v>
+      </c>
+      <c r="U11" s="78"/>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
@@ -2080,7 +2278,17 @@
       <c r="I12" s="5">
         <v>0</v>
       </c>
+      <c r="J12" s="67">
+        <f t="shared" ref="J12:J13" si="3">T12-I12</f>
+        <v>0</v>
+      </c>
       <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="T12" s="5">
         <v>0</v>
       </c>
     </row>
@@ -2091,8 +2299,18 @@
       <c r="I13" s="5">
         <v>0.86</v>
       </c>
+      <c r="J13" s="67">
+        <f t="shared" si="3"/>
+        <v>0.69800000000000006</v>
+      </c>
       <c r="K13" s="5">
         <v>0.59899999999999998</v>
+      </c>
+      <c r="S13" s="5">
+        <v>1.901</v>
+      </c>
+      <c r="T13" s="5">
+        <v>1.5580000000000001</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.15">
@@ -2103,10 +2321,22 @@
         <f>I11+I12-I13</f>
         <v>-2.6119999999999997</v>
       </c>
+      <c r="J14" s="71">
+        <f>J11+J12-J13</f>
+        <v>12.067999999999994</v>
+      </c>
       <c r="K14" s="5">
         <f>K11+K12-K13</f>
         <v>3.0620000000000047</v>
       </c>
+      <c r="S14" s="5">
+        <f t="shared" ref="S14:T14" si="4">S11+S12-S13</f>
+        <v>-14.600999999999997</v>
+      </c>
+      <c r="T14" s="5">
+        <f t="shared" si="4"/>
+        <v>9.455999999999996</v>
+      </c>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
@@ -2115,8 +2345,18 @@
       <c r="I15" s="5">
         <v>-0.497</v>
       </c>
+      <c r="J15" s="67">
+        <f>T15-I15</f>
+        <v>2.9390000000000001</v>
+      </c>
       <c r="K15" s="5">
         <v>0.19700000000000001</v>
+      </c>
+      <c r="S15" s="5">
+        <v>-2.698</v>
+      </c>
+      <c r="T15" s="5">
+        <v>2.4420000000000002</v>
       </c>
     </row>
     <row r="16" spans="2:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -2130,25 +2370,73 @@
         <f>I14-I15</f>
         <v>-2.1149999999999998</v>
       </c>
-      <c r="J16" s="30"/>
+      <c r="J16" s="69">
+        <f>J14-J15</f>
+        <v>9.1289999999999942</v>
+      </c>
       <c r="K16" s="31">
         <f>K14-K15</f>
         <v>2.8650000000000047</v>
       </c>
       <c r="L16" s="30"/>
       <c r="N16" s="30"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="S16" s="31">
+        <f t="shared" ref="S16:T16" si="5">S14-S15</f>
+        <v>-11.902999999999997</v>
+      </c>
+      <c r="T16" s="31">
+        <f t="shared" si="5"/>
+        <v>7.0139999999999958</v>
+      </c>
+      <c r="U16" s="78"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="I17" s="56">
+        <f>I16/I18</f>
+        <v>-4.2299999999999997E-2</v>
+      </c>
+      <c r="J17" s="57">
+        <f>J16/J18</f>
+        <v>0.18257999999999988</v>
+      </c>
+      <c r="K17" s="56">
+        <f>K16/K18</f>
+        <v>5.7300000000000094E-2</v>
+      </c>
+      <c r="S17" s="56">
+        <f t="shared" ref="S17:T17" si="6">S16/S18</f>
+        <v>-0.23805999999999994</v>
+      </c>
+      <c r="T17" s="56">
+        <f t="shared" si="6"/>
+        <v>0.1402799999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="2:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I18" s="53">
+        <v>50</v>
+      </c>
+      <c r="J18" s="70">
+        <f>T18</f>
+        <v>50</v>
+      </c>
+      <c r="K18" s="53">
+        <v>50</v>
+      </c>
+      <c r="S18" s="53">
+        <v>50</v>
+      </c>
+      <c r="T18" s="53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>75</v>
       </c>
@@ -2162,8 +2450,15 @@
       </c>
       <c r="L21" s="30"/>
       <c r="N21" s="30"/>
-    </row>
-    <row r="22" spans="2:14" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="T21" s="32">
+        <f>T6/S6-1</f>
+        <v>-2.7951830820442503E-2</v>
+      </c>
+      <c r="U21" s="79">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="39" t="s">
         <v>114</v>
       </c>
@@ -2177,8 +2472,13 @@
       </c>
       <c r="L22" s="37"/>
       <c r="N22" s="37"/>
-    </row>
-    <row r="23" spans="2:14" s="36" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="T22" s="42">
+        <f>T4/S4-1</f>
+        <v>-0.13980582524271845</v>
+      </c>
+      <c r="U22" s="74"/>
+    </row>
+    <row r="23" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B23" s="39" t="s">
         <v>115</v>
       </c>
@@ -2192,13 +2492,38 @@
       </c>
       <c r="L23" s="37"/>
       <c r="N23" s="37"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="T23" s="42">
+        <f>T5/S5-1</f>
+        <v>0.58031088082901539</v>
+      </c>
+      <c r="U23" s="74"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="J24" s="34">
+        <f t="shared" ref="J24" si="7">J6/I6-1</f>
+        <v>0.94650673921107931</v>
+      </c>
+      <c r="K24" s="33">
+        <f>K6/J6-1</f>
+        <v>-0.11235341202180227</v>
+      </c>
+      <c r="Q24" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="R24" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="S24" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="T24" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B26" s="33" t="s">
         <v>77</v>
       </c>
@@ -2209,15 +2534,27 @@
         <f>I8/I6</f>
         <v>0.19159144305675774</v>
       </c>
-      <c r="J26" s="34"/>
+      <c r="J26" s="34">
+        <f>J8/J6</f>
+        <v>0.31417790031382209</v>
+      </c>
       <c r="K26" s="33">
         <f>K8/K6</f>
         <v>0.19490724836825837</v>
       </c>
       <c r="L26" s="34"/>
       <c r="N26" s="34"/>
-    </row>
-    <row r="27" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S26" s="33">
+        <f>S8/S6</f>
+        <v>4.2719143659030123E-2</v>
+      </c>
+      <c r="T26" s="33">
+        <f>T8/T6</f>
+        <v>0.27257390340937698</v>
+      </c>
+      <c r="U26" s="80"/>
+    </row>
+    <row r="27" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B27" s="33" t="s">
         <v>78</v>
       </c>
@@ -2228,15 +2565,27 @@
         <f>I11/I6</f>
         <v>-4.3328799307530599E-2</v>
       </c>
-      <c r="J27" s="34"/>
+      <c r="J27" s="34">
+        <f>J11/J6</f>
+        <v>0.16219650094654853</v>
+      </c>
       <c r="K27" s="33">
         <f>K11/K6</f>
         <v>5.2401809229359962E-2</v>
       </c>
       <c r="L27" s="34"/>
       <c r="N27" s="34"/>
-    </row>
-    <row r="28" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S27" s="33">
+        <f>S11/S6</f>
+        <v>-0.10369753932510931</v>
+      </c>
+      <c r="T27" s="33">
+        <f>T11/T6</f>
+        <v>9.2444310150912326E-2</v>
+      </c>
+      <c r="U27" s="80"/>
+    </row>
+    <row r="28" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B28" s="33" t="s">
         <v>79</v>
       </c>
@@ -2247,15 +2596,27 @@
         <f>I16/I6</f>
         <v>-5.2306170396933339E-2</v>
       </c>
-      <c r="J28" s="34"/>
+      <c r="J28" s="34">
+        <f>J16/J6</f>
+        <v>0.11598714218557428</v>
+      </c>
       <c r="K28" s="33">
         <f>K16/K6</f>
         <v>4.1008244589488214E-2</v>
       </c>
       <c r="L28" s="34"/>
       <c r="N28" s="34"/>
-    </row>
-    <row r="29" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S28" s="33">
+        <f>S16/S6</f>
+        <v>-9.7113439070556723E-2</v>
+      </c>
+      <c r="T28" s="33">
+        <f>T16/T6</f>
+        <v>5.8870927128972114E-2</v>
+      </c>
+      <c r="U28" s="80"/>
+    </row>
+    <row r="29" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B29" s="33" t="s">
         <v>80</v>
       </c>
@@ -2266,31 +2627,45 @@
         <f>I15/I14</f>
         <v>0.1902756508422665</v>
       </c>
-      <c r="J29" s="34"/>
+      <c r="J29" s="34">
+        <f>J15/J14</f>
+        <v>0.24353662578720595</v>
+      </c>
       <c r="K29" s="33">
         <f>K15/K14</f>
         <v>6.4337034617896707E-2</v>
       </c>
       <c r="L29" s="34"/>
       <c r="N29" s="34"/>
-    </row>
-    <row r="30" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S29" s="33">
+        <f>S15/S14</f>
+        <v>0.18478186425587292</v>
+      </c>
+      <c r="T29" s="33">
+        <f>T15/T14</f>
+        <v>0.25824873096446715</v>
+      </c>
+      <c r="U29" s="80"/>
+    </row>
+    <row r="30" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D30" s="34"/>
       <c r="F30" s="34"/>
       <c r="H30" s="34"/>
       <c r="J30" s="34"/>
       <c r="L30" s="34"/>
       <c r="N30" s="34"/>
-    </row>
-    <row r="31" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="U30" s="80"/>
+    </row>
+    <row r="31" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="D31" s="34"/>
       <c r="F31" s="34"/>
       <c r="H31" s="34"/>
       <c r="J31" s="34"/>
       <c r="L31" s="34"/>
       <c r="N31" s="34"/>
-    </row>
-    <row r="32" spans="2:14" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="U31" s="80"/>
+    </row>
+    <row r="32" spans="2:21" s="33" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B32" s="41" t="s">
         <v>109</v>
       </c>
@@ -2300,16 +2675,20 @@
       <c r="J32" s="34"/>
       <c r="L32" s="34"/>
       <c r="N32" s="34"/>
-    </row>
-    <row r="33" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="U32" s="80"/>
+    </row>
+    <row r="33" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
         <v>110</v>
       </c>
       <c r="D33" s="30"/>
       <c r="F33" s="30"/>
-      <c r="H33" s="30"/>
+      <c r="H33" s="30">
+        <f>S33</f>
+        <v>460</v>
+      </c>
       <c r="J33" s="30">
-        <f t="shared" ref="J33" si="0">J34+J35+J36</f>
+        <f t="shared" ref="J33" si="8">J34+J35+J36</f>
         <v>410</v>
       </c>
       <c r="K33" s="2">
@@ -2318,125 +2697,194 @@
       </c>
       <c r="L33" s="30"/>
       <c r="N33" s="30"/>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S33" s="2">
+        <f>S34+S35+S36</f>
+        <v>460</v>
+      </c>
+      <c r="T33" s="2">
+        <f>T34+T35+T36</f>
+        <v>410</v>
+      </c>
+      <c r="U33" s="78"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B34" s="38" t="s">
         <v>111</v>
       </c>
+      <c r="H34" s="25">
+        <f>S34</f>
+        <v>51</v>
+      </c>
       <c r="J34" s="25">
         <v>45</v>
       </c>
       <c r="K34" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S34" s="1">
+        <v>51</v>
+      </c>
+      <c r="T34" s="1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B35" s="38" t="s">
         <v>112</v>
       </c>
+      <c r="H35" s="25">
+        <f>S35</f>
+        <v>6</v>
+      </c>
       <c r="J35" s="25">
         <v>22</v>
       </c>
       <c r="K35" s="1">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S35" s="1">
+        <v>6</v>
+      </c>
+      <c r="T35" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B36" s="38" t="s">
         <v>113</v>
       </c>
+      <c r="H36" s="25">
+        <f>S36</f>
+        <v>403</v>
+      </c>
       <c r="J36" s="25">
         <v>343</v>
       </c>
       <c r="K36" s="1">
         <v>308</v>
       </c>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S36" s="68">
+        <v>403</v>
+      </c>
+      <c r="T36" s="1">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B38" s="35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="H39" s="71">
+        <f>S39</f>
+        <v>16.966999999999999</v>
+      </c>
       <c r="I39" s="5">
         <v>14.733000000000001</v>
       </c>
-      <c r="J39" s="25">
+      <c r="J39" s="71">
         <f>T39</f>
-        <v>0</v>
+        <v>14.227</v>
       </c>
       <c r="K39" s="5">
         <v>13.555</v>
       </c>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S39" s="5">
+        <v>16.966999999999999</v>
+      </c>
+      <c r="T39" s="5">
+        <v>14.227</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="H40" s="71">
+        <f t="shared" ref="H40:H41" si="9">S40</f>
+        <v>42.387</v>
+      </c>
       <c r="I40" s="5">
         <v>36.463999999999999</v>
       </c>
-      <c r="J40" s="25">
-        <f t="shared" ref="J40:J41" si="1">T40</f>
-        <v>0</v>
+      <c r="J40" s="71">
+        <f t="shared" ref="J40:J41" si="10">T40</f>
+        <v>30.884</v>
       </c>
       <c r="K40" s="5">
         <v>28.526</v>
       </c>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S40" s="5">
+        <v>42.387</v>
+      </c>
+      <c r="T40" s="5">
+        <v>30.884</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="H41" s="71">
+        <f t="shared" si="9"/>
+        <v>5.617</v>
+      </c>
       <c r="I41" s="5">
         <v>5.4550000000000001</v>
       </c>
-      <c r="J41" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="J41" s="71">
+        <f t="shared" si="10"/>
+        <v>3.22</v>
       </c>
       <c r="K41" s="5">
         <v>2.4900000000000002</v>
       </c>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S41" s="5">
+        <v>5.617</v>
+      </c>
+      <c r="T41" s="5">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ref="C42:J42" si="2">SUM(C39:C41)</f>
+        <f t="shared" ref="C42:J42" si="11">SUM(C39:C41)</f>
         <v>0</v>
       </c>
       <c r="D42" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="F42" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="G42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="H42" s="25">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>64.971000000000004</v>
       </c>
       <c r="I42" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="11"/>
         <v>56.652000000000001</v>
       </c>
-      <c r="J42" s="25">
-        <f t="shared" si="2"/>
-        <v>0</v>
+      <c r="J42" s="71">
+        <f t="shared" si="11"/>
+        <v>48.331000000000003</v>
       </c>
       <c r="K42" s="5">
         <f>SUM(K39:K41)</f>
@@ -2450,120 +2898,160 @@
         <f>SUM(R39:R41)</f>
         <v>0</v>
       </c>
-      <c r="S42" s="1">
+      <c r="S42" s="5">
         <f>SUM(S39:S41)</f>
-        <v>0</v>
-      </c>
-      <c r="T42" s="1">
+        <v>64.971000000000004</v>
+      </c>
+      <c r="T42" s="5">
         <f>SUM(T39:T41)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+        <v>48.331000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B43" s="2" t="s">
         <v>86</v>
       </c>
       <c r="D43" s="30"/>
       <c r="F43" s="30"/>
-      <c r="H43" s="30"/>
+      <c r="H43" s="69">
+        <f>S43</f>
+        <v>26.698</v>
+      </c>
       <c r="I43" s="31">
         <v>28.433</v>
       </c>
-      <c r="J43" s="30">
+      <c r="J43" s="69">
         <f>T43</f>
-        <v>0</v>
+        <v>25.131</v>
       </c>
       <c r="K43" s="31">
         <v>31.096</v>
       </c>
       <c r="L43" s="30"/>
       <c r="N43" s="30"/>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S43" s="31">
+        <v>26.698</v>
+      </c>
+      <c r="T43" s="31">
+        <v>25.131</v>
+      </c>
+      <c r="U43" s="78"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="H44" s="71">
+        <f t="shared" ref="H44:H45" si="12">S44</f>
+        <v>2.7349999999999999</v>
+      </c>
       <c r="I44" s="5">
         <v>3.524</v>
       </c>
-      <c r="J44" s="25">
-        <f t="shared" ref="J44:J45" si="3">T44</f>
-        <v>0</v>
+      <c r="J44" s="71">
+        <f t="shared" ref="J44" si="13">T44</f>
+        <v>5.4569999999999999</v>
       </c>
       <c r="K44" s="5">
         <v>3.45</v>
       </c>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S44" s="5">
+        <v>2.7349999999999999</v>
+      </c>
+      <c r="T44" s="5">
+        <v>5.4569999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="H45" s="71">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
       <c r="I45" s="5">
         <v>0</v>
       </c>
-      <c r="J45" s="25">
-        <f t="shared" si="3"/>
+      <c r="J45" s="71">
+        <f>T45</f>
         <v>0</v>
       </c>
       <c r="K45" s="5">
         <v>0.45600000000000002</v>
       </c>
-    </row>
-    <row r="46" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S45" s="5">
+        <v>0</v>
+      </c>
+      <c r="T45" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D46" s="30"/>
       <c r="F46" s="30"/>
-      <c r="H46" s="30"/>
+      <c r="H46" s="69">
+        <f>S46</f>
+        <v>13.266</v>
+      </c>
       <c r="I46" s="31">
         <v>14.473000000000001</v>
       </c>
-      <c r="J46" s="30">
+      <c r="J46" s="69">
         <f>T46</f>
-        <v>0</v>
+        <v>19.015000000000001</v>
       </c>
       <c r="K46" s="31">
         <v>13.872</v>
       </c>
       <c r="L46" s="30"/>
       <c r="N46" s="30"/>
-    </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S46" s="31">
+        <v>13.266</v>
+      </c>
+      <c r="T46" s="31">
+        <v>19.015000000000001</v>
+      </c>
+      <c r="U46" s="78"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" ref="C47:J47" si="4">SUM(C43:C46)+C42</f>
+        <f t="shared" ref="C47:J47" si="14">SUM(C43:C46)+C42</f>
         <v>0</v>
       </c>
       <c r="D47" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="F47" s="25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H47" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="14"/>
+        <v>107.67</v>
       </c>
       <c r="I47" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>103.08199999999999</v>
       </c>
-      <c r="J47" s="25">
-        <f t="shared" si="4"/>
-        <v>0</v>
+      <c r="J47" s="71">
+        <f t="shared" si="14"/>
+        <v>97.933999999999997</v>
       </c>
       <c r="K47" s="5">
         <f>SUM(K43:K46)+K42</f>
@@ -2577,70 +3065,103 @@
         <f>SUM(R43:R46)+R42</f>
         <v>0</v>
       </c>
-      <c r="S47" s="1">
+      <c r="S47" s="5">
         <f>SUM(S43:S46)+S42</f>
-        <v>0</v>
-      </c>
-      <c r="T47" s="1">
+        <v>107.67</v>
+      </c>
+      <c r="T47" s="5">
         <f>SUM(T43:T46)+T42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.15">
+        <v>97.933999999999997</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.15">
       <c r="I48" s="5"/>
+      <c r="J48" s="71"/>
       <c r="K48" s="5"/>
-    </row>
-    <row r="49" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="H49" s="71">
+        <f t="shared" ref="H49:H50" si="15">S49</f>
+        <v>17.315999999999999</v>
+      </c>
       <c r="I49" s="5">
         <v>12.25</v>
       </c>
-      <c r="J49" s="25">
-        <f t="shared" ref="J49:J50" si="5">T49</f>
-        <v>0</v>
+      <c r="J49" s="71">
+        <f t="shared" ref="J49:J50" si="16">T49</f>
+        <v>16.440000000000001</v>
       </c>
       <c r="K49" s="5">
         <v>19.484000000000002</v>
       </c>
-    </row>
-    <row r="50" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S49" s="5">
+        <v>17.315999999999999</v>
+      </c>
+      <c r="T49" s="5">
+        <v>16.440000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="H50" s="71">
+        <f t="shared" si="15"/>
+        <v>19.914000000000001</v>
+      </c>
       <c r="I50" s="5">
         <v>15.629</v>
       </c>
-      <c r="J50" s="25">
-        <f t="shared" si="5"/>
-        <v>0</v>
+      <c r="J50" s="71">
+        <f t="shared" si="16"/>
+        <v>17.035</v>
       </c>
       <c r="K50" s="5">
         <v>14.016</v>
       </c>
-    </row>
-    <row r="51" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S50" s="5">
+        <v>19.914000000000001</v>
+      </c>
+      <c r="T50" s="5">
+        <v>17.035</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B51" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D51" s="30"/>
       <c r="F51" s="30"/>
-      <c r="H51" s="30"/>
+      <c r="H51" s="69">
+        <f>S51</f>
+        <v>0.105</v>
+      </c>
       <c r="I51" s="31">
         <v>2.62</v>
       </c>
-      <c r="J51" s="30">
-        <f t="shared" ref="J51:J54" si="6">T51</f>
-        <v>0</v>
+      <c r="J51" s="69">
+        <f t="shared" ref="J51:J54" si="17">T51</f>
+        <v>0.59099999999999997</v>
       </c>
       <c r="K51" s="31">
         <v>0</v>
       </c>
       <c r="L51" s="30"/>
       <c r="N51" s="30"/>
-    </row>
-    <row r="52" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S51" s="31">
+        <v>0.105</v>
+      </c>
+      <c r="T51" s="31">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="U51" s="78"/>
+    </row>
+    <row r="52" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B52" s="2" t="s">
         <v>93</v>
       </c>
@@ -2650,81 +3171,108 @@
       <c r="I52" s="31">
         <v>4.8</v>
       </c>
-      <c r="J52" s="30">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="J52" s="69">
+        <f t="shared" si="17"/>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K52" s="31">
         <v>0</v>
       </c>
       <c r="L52" s="30"/>
       <c r="N52" s="30"/>
-    </row>
-    <row r="53" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S52" s="31">
+        <v>1.944</v>
+      </c>
+      <c r="T52" s="31">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="U52" s="78"/>
+    </row>
+    <row r="53" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="H53" s="71">
+        <f t="shared" ref="H53:H54" si="18">S53</f>
+        <v>1.4710000000000001</v>
+      </c>
       <c r="I53" s="5">
         <v>1.756</v>
       </c>
-      <c r="J53" s="25">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="J53" s="71">
+        <f t="shared" si="17"/>
+        <v>1.698</v>
       </c>
       <c r="K53" s="5">
         <v>1.7270000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S53" s="5">
+        <v>1.4710000000000001</v>
+      </c>
+      <c r="T53" s="5">
+        <v>1.698</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="H54" s="71">
+        <f t="shared" si="18"/>
+        <v>0.13700000000000001</v>
+      </c>
       <c r="I54" s="5">
         <v>0</v>
       </c>
-      <c r="J54" s="25">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="J54" s="71">
+        <f t="shared" si="17"/>
+        <v>0.77300000000000002</v>
       </c>
       <c r="K54" s="5">
         <v>0.317</v>
       </c>
-    </row>
-    <row r="55" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S54" s="5">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="T54" s="5">
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" ref="C55:J55" si="7">SUM(C49:C54)</f>
+        <f t="shared" ref="C55:J55" si="19">SUM(C49:C54)</f>
         <v>0</v>
       </c>
       <c r="D55" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="F55" s="25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="G55" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="H55" s="25">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>38.942999999999998</v>
       </c>
       <c r="I55" s="5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="19"/>
         <v>37.055</v>
       </c>
-      <c r="J55" s="25">
-        <f t="shared" si="7"/>
-        <v>0</v>
+      <c r="J55" s="71">
+        <f t="shared" si="19"/>
+        <v>40.937000000000005</v>
       </c>
       <c r="K55" s="5">
         <f>SUM(K49:K54)</f>
@@ -2738,42 +3286,55 @@
         <f>SUM(R49:R54)</f>
         <v>0</v>
       </c>
-      <c r="S55" s="1">
+      <c r="S55" s="5">
         <f>SUM(S49:S54)</f>
-        <v>0</v>
-      </c>
-      <c r="T55" s="1">
+        <v>40.887</v>
+      </c>
+      <c r="T55" s="5">
         <f>SUM(T49:T54)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:20" x14ac:dyDescent="0.15">
+        <v>40.937000000000005</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="H56" s="71">
+        <f>S56</f>
+        <v>37.475000000000001</v>
+      </c>
       <c r="I56" s="5">
         <v>40.042000000000002</v>
       </c>
-      <c r="J56" s="25">
+      <c r="J56" s="71">
         <f>T56</f>
-        <v>0</v>
+        <v>25.942</v>
       </c>
       <c r="K56" s="5">
         <v>23.553999999999998</v>
       </c>
-    </row>
-    <row r="57" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="S56" s="5">
+        <v>37.475000000000001</v>
+      </c>
+      <c r="T56" s="5">
+        <v>25.942</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B57" s="2" t="s">
         <v>93</v>
       </c>
       <c r="D57" s="30"/>
       <c r="F57" s="30"/>
-      <c r="H57" s="30"/>
+      <c r="H57" s="69">
+        <f>S57</f>
+        <v>5.056</v>
+      </c>
       <c r="I57" s="31">
         <v>5.6</v>
       </c>
-      <c r="J57" s="30">
-        <f t="shared" ref="J57:J59" si="8">T57</f>
+      <c r="J57" s="69">
+        <f t="shared" ref="J57:J59" si="20">T57</f>
         <v>0</v>
       </c>
       <c r="K57" s="31">
@@ -2781,72 +3342,99 @@
       </c>
       <c r="L57" s="30"/>
       <c r="N57" s="30"/>
-    </row>
-    <row r="58" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S57" s="31">
+        <v>5.056</v>
+      </c>
+      <c r="T57" s="31">
+        <v>0</v>
+      </c>
+      <c r="U57" s="78"/>
+    </row>
+    <row r="58" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="H58" s="71">
+        <f t="shared" ref="H58:H59" si="21">S58</f>
+        <v>1.26</v>
+      </c>
       <c r="I58" s="5">
         <v>1.4990000000000001</v>
       </c>
-      <c r="J58" s="25">
-        <f t="shared" si="8"/>
-        <v>0</v>
+      <c r="J58" s="71">
+        <f t="shared" si="20"/>
+        <v>1.728</v>
       </c>
       <c r="K58" s="5">
         <v>2.0840000000000001</v>
       </c>
-    </row>
-    <row r="59" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S58" s="5">
+        <v>1.26</v>
+      </c>
+      <c r="T58" s="5">
+        <v>1.728</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="H59" s="71">
+        <f t="shared" si="21"/>
+        <v>10.593999999999999</v>
+      </c>
       <c r="I59" s="5">
         <v>7.899</v>
       </c>
-      <c r="J59" s="25">
-        <f t="shared" si="8"/>
-        <v>0</v>
+      <c r="J59" s="71">
+        <f t="shared" si="20"/>
+        <v>5.9089999999999998</v>
       </c>
       <c r="K59" s="5">
         <v>2.8570000000000002</v>
       </c>
-    </row>
-    <row r="60" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="S59" s="5">
+        <v>10.593999999999999</v>
+      </c>
+      <c r="T59" s="5">
+        <v>5.9089999999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
         <v>98</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" ref="C60:J60" si="9">C55+SUM(C56:C59)</f>
+        <f t="shared" ref="C60:J60" si="22">C55+SUM(C56:C59)</f>
         <v>0</v>
       </c>
       <c r="D60" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="F60" s="25">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H60" s="25">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>93.328000000000003</v>
       </c>
       <c r="I60" s="5">
-        <f t="shared" si="9"/>
+        <f t="shared" si="22"/>
         <v>92.094999999999999</v>
       </c>
-      <c r="J60" s="25">
-        <f t="shared" si="9"/>
-        <v>0</v>
+      <c r="J60" s="71">
+        <f t="shared" si="22"/>
+        <v>74.516000000000005</v>
       </c>
       <c r="K60" s="5">
         <f>K55+SUM(K56:K59)</f>
@@ -2860,53 +3448,56 @@
         <f>R55+SUM(R56:R59)</f>
         <v>0</v>
       </c>
-      <c r="S60" s="1">
+      <c r="S60" s="5">
         <f>S55+SUM(S56:S59)</f>
-        <v>0</v>
-      </c>
-      <c r="T60" s="1">
+        <v>95.271999999999991</v>
+      </c>
+      <c r="T60" s="5">
         <f>T55+SUM(T56:T59)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:20" x14ac:dyDescent="0.15">
+        <v>74.516000000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" x14ac:dyDescent="0.15">
       <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="J61" s="71"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+    </row>
+    <row r="62" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B62" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" ref="C62:J62" si="10">C47-C60</f>
+        <f t="shared" ref="C62:J62" si="23">C47-C60</f>
         <v>0</v>
       </c>
       <c r="D62" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F62" s="25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G62" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H62" s="25">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>14.341999999999999</v>
       </c>
       <c r="I62" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="23"/>
         <v>10.986999999999995</v>
       </c>
-      <c r="J62" s="25">
-        <f t="shared" si="10"/>
-        <v>0</v>
+      <c r="J62" s="71">
+        <f t="shared" si="23"/>
+        <v>23.417999999999992</v>
       </c>
       <c r="K62" s="53">
         <f>K47-K60</f>
@@ -2920,50 +3511,50 @@
         <f>R47-R60</f>
         <v>0</v>
       </c>
-      <c r="S62" s="1">
+      <c r="S62" s="5">
         <f>S47-S60</f>
-        <v>0</v>
-      </c>
-      <c r="T62" s="1">
+        <v>12.39800000000001</v>
+      </c>
+      <c r="T62" s="5">
         <f>T47-T60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:20" x14ac:dyDescent="0.15">
+        <v>23.417999999999992</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B63" s="1" t="s">
         <v>100</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" ref="C63:J63" si="11">C62+C60</f>
+        <f t="shared" ref="C63:J63" si="24">C62+C60</f>
         <v>0</v>
       </c>
       <c r="D63" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="F63" s="25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H63" s="25">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="24"/>
+        <v>107.67</v>
       </c>
       <c r="I63" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="24"/>
         <v>103.08199999999999</v>
       </c>
-      <c r="J63" s="25">
-        <f t="shared" si="11"/>
-        <v>0</v>
+      <c r="J63" s="71">
+        <f t="shared" si="24"/>
+        <v>97.933999999999997</v>
       </c>
       <c r="K63" s="53">
         <f>K62+K60</f>
@@ -2977,53 +3568,55 @@
         <f>R62+R60</f>
         <v>0</v>
       </c>
-      <c r="S63" s="1">
+      <c r="S63" s="5">
         <f>S62+S60</f>
-        <v>0</v>
-      </c>
-      <c r="T63" s="1">
+        <v>107.67</v>
+      </c>
+      <c r="T63" s="5">
         <f>T62+T60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:20" x14ac:dyDescent="0.15">
+        <v>97.933999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="2:21" x14ac:dyDescent="0.15">
       <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="J64" s="71"/>
+      <c r="T64" s="5"/>
+    </row>
+    <row r="65" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C65" s="1">
-        <f t="shared" ref="C65:J65" si="12">C47-C60</f>
+        <f t="shared" ref="C65:J65" si="25">C47-C60</f>
         <v>0</v>
       </c>
       <c r="D65" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="E65" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="F65" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="G65" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="H65" s="25">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>14.341999999999999</v>
       </c>
       <c r="I65" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="25"/>
         <v>10.986999999999995</v>
       </c>
-      <c r="J65" s="25">
-        <f t="shared" si="12"/>
-        <v>0</v>
+      <c r="J65" s="71">
+        <f t="shared" si="25"/>
+        <v>23.417999999999992</v>
       </c>
       <c r="K65" s="53">
         <f>K47-K60</f>
@@ -3039,56 +3632,76 @@
       </c>
       <c r="S65" s="1">
         <f>S47-S60</f>
-        <v>0</v>
-      </c>
-      <c r="T65" s="1">
+        <v>12.39800000000001</v>
+      </c>
+      <c r="T65" s="5">
         <f>T47-T60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:20" x14ac:dyDescent="0.15">
+        <v>23.417999999999992</v>
+      </c>
+    </row>
+    <row r="66" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B66" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="67" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="I66" s="1">
+        <f>I65/I18</f>
+        <v>0.21973999999999991</v>
+      </c>
+      <c r="J66" s="25">
+        <f>J65/J18</f>
+        <v>0.46835999999999983</v>
+      </c>
+      <c r="K66" s="1">
+        <f>K65/K18</f>
+        <v>0.58812000000000042</v>
+      </c>
+      <c r="S66" s="1">
+        <f>S65/S18</f>
+        <v>0.24796000000000021</v>
+      </c>
+      <c r="T66" s="1">
+        <f>T65/T18</f>
+        <v>0.46835999999999983</v>
+      </c>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.15">
       <c r="K67" s="5"/>
     </row>
-    <row r="68" spans="2:20" s="36" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B68" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="36">
-        <f t="shared" ref="C68:J68" si="13">C46</f>
+        <f t="shared" ref="C68:J68" si="26">C46</f>
         <v>0</v>
       </c>
       <c r="D68" s="37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="E68" s="36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="F68" s="37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="G68" s="36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="H68" s="37">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>13.266</v>
       </c>
       <c r="I68" s="39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="26"/>
         <v>14.473000000000001</v>
       </c>
       <c r="J68" s="37">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>19.015000000000001</v>
       </c>
       <c r="K68" s="39">
         <f>K46</f>
@@ -3106,48 +3719,49 @@
       </c>
       <c r="S68" s="36">
         <f>S46</f>
-        <v>0</v>
+        <v>13.266</v>
       </c>
       <c r="T68" s="36">
         <f>T46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:20" s="36" customFormat="1" x14ac:dyDescent="0.15">
+        <v>19.015000000000001</v>
+      </c>
+      <c r="U68" s="74"/>
+    </row>
+    <row r="69" spans="2:21" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B69" s="36" t="s">
         <v>7</v>
       </c>
       <c r="C69" s="36">
-        <f t="shared" ref="C69:J69" si="14">C51+C52+C57</f>
+        <f t="shared" ref="C69:J69" si="27">C51+C52+C57</f>
         <v>0</v>
       </c>
       <c r="D69" s="37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="E69" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="F69" s="37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G69" s="36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="H69" s="37">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>5.1610000000000005</v>
       </c>
       <c r="I69" s="39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="27"/>
         <v>13.02</v>
       </c>
       <c r="J69" s="37">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>4.9910000000000005</v>
       </c>
       <c r="K69" s="39">
         <f>K51+K52+K57</f>
@@ -3165,48 +3779,49 @@
       </c>
       <c r="S69" s="36">
         <f>S51+S52+S57</f>
-        <v>0</v>
+        <v>7.1050000000000004</v>
       </c>
       <c r="T69" s="36">
         <f>T51+T52+T57</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:20" x14ac:dyDescent="0.15">
+        <v>4.9910000000000005</v>
+      </c>
+      <c r="U69" s="74"/>
+    </row>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B70" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="1">
-        <f t="shared" ref="C70:J70" si="15">C68-C69</f>
+        <f t="shared" ref="C70:J70" si="28">C68-C69</f>
         <v>0</v>
       </c>
       <c r="D70" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="F70" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="G70" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H70" s="25">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>8.1050000000000004</v>
       </c>
       <c r="I70" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="28"/>
         <v>1.4530000000000012</v>
       </c>
       <c r="J70" s="25">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>14.024000000000001</v>
       </c>
       <c r="K70" s="5">
         <f>K68-K69</f>
@@ -3222,45 +3837,205 @@
       </c>
       <c r="S70" s="1">
         <f>S68-S69</f>
-        <v>0</v>
+        <v>6.1609999999999996</v>
       </c>
       <c r="T70" s="1">
         <f>T68-T69</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="B72" s="1" t="s">
+        <v>14.024000000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B72" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K72" s="33">
+      <c r="D72" s="30"/>
+      <c r="F72" s="30"/>
+      <c r="H72" s="30"/>
+      <c r="J72" s="30"/>
+      <c r="K72" s="32">
         <f>K43/I43-1</f>
         <v>9.3658776773467567E-2</v>
       </c>
-    </row>
-    <row r="73" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="L72" s="30"/>
+      <c r="N72" s="30"/>
+      <c r="U72" s="78"/>
+    </row>
+    <row r="73" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B73" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="74" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="J73" s="34">
+        <f>J43/I43-1</f>
+        <v>-0.11613266275102874</v>
+      </c>
+      <c r="K73" s="33">
+        <f>K43/J43-1</f>
+        <v>0.23735625323305887</v>
+      </c>
+    </row>
+    <row r="74" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B74" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="B76" s="1" t="s">
+    <row r="76" spans="2:21" s="58" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="58" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="77" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="D76" s="59"/>
+      <c r="F76" s="59"/>
+      <c r="H76" s="59">
+        <f>S76</f>
+        <v>0.436</v>
+      </c>
+      <c r="I76" s="58">
+        <v>0.63949999999999996</v>
+      </c>
+      <c r="J76" s="59">
+        <f>T76</f>
+        <v>0.63949999999999996</v>
+      </c>
+      <c r="K76" s="58">
+        <v>1.3564000000000001</v>
+      </c>
+      <c r="L76" s="59"/>
+      <c r="N76" s="59"/>
+      <c r="S76" s="58">
+        <v>0.436</v>
+      </c>
+      <c r="T76" s="58">
+        <v>0.63949999999999996</v>
+      </c>
+      <c r="U76" s="81"/>
+    </row>
+    <row r="77" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B77" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="I77" s="5">
+        <f>I76*I18</f>
+        <v>31.974999999999998</v>
+      </c>
+      <c r="J77" s="71">
+        <f>J76*J18</f>
+        <v>31.974999999999998</v>
+      </c>
+      <c r="K77" s="5">
+        <f>K76*K18</f>
+        <v>67.820000000000007</v>
+      </c>
+      <c r="S77" s="5">
+        <f t="shared" ref="S77" si="29">S76*S18</f>
+        <v>21.8</v>
+      </c>
+      <c r="T77" s="5">
+        <f>T76*T18</f>
+        <v>31.974999999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B78" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="I78" s="5">
+        <f>I77-I70</f>
+        <v>30.521999999999998</v>
+      </c>
+      <c r="J78" s="71">
+        <f>J77-J70</f>
+        <v>17.950999999999997</v>
+      </c>
+      <c r="K78" s="5">
+        <f>K77-K70</f>
+        <v>53.948000000000008</v>
+      </c>
+      <c r="S78" s="5">
+        <f t="shared" ref="S78" si="30">S77-S70</f>
+        <v>15.639000000000001</v>
+      </c>
+      <c r="T78" s="5">
+        <f>T77-T70</f>
+        <v>17.950999999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="2:21" s="60" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B80" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="D80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="H80" s="61"/>
+      <c r="I80" s="60">
+        <f>I76/I66</f>
+        <v>2.9102575771366168</v>
+      </c>
+      <c r="J80" s="61">
+        <f>J76/J66</f>
+        <v>1.3654026816978397</v>
+      </c>
+      <c r="K80" s="60">
+        <f>K76/K66</f>
+        <v>2.3063320410800503</v>
+      </c>
+      <c r="L80" s="61"/>
+      <c r="N80" s="61"/>
+      <c r="S80" s="60">
+        <f t="shared" ref="S80:T80" si="31">S76/S66</f>
+        <v>1.7583481206646219</v>
+      </c>
+      <c r="T80" s="60">
+        <f>T76/T66</f>
+        <v>1.3654026816978397</v>
+      </c>
+      <c r="U80" s="82"/>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="B81" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J81" s="61">
+        <f>J77/SUM(I6:J6)</f>
+        <v>0.26837723053163454</v>
+      </c>
+      <c r="K81" s="60">
+        <f>K77/SUM(J6:K6)</f>
+        <v>0.45648208600601736</v>
+      </c>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="B82" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="B83" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J83" s="61">
+        <f>J76/SUM(I17:J17)</f>
+        <v>4.5587396635300861</v>
+      </c>
+      <c r="K83" s="60">
+        <f>K76/SUM(J17:K17)</f>
+        <v>5.6544939136234786</v>
+      </c>
+      <c r="S83" s="60">
+        <f t="shared" ref="S83:T83" si="32">S76/S17</f>
+        <v>-1.8314710577165425</v>
+      </c>
+      <c r="T83" s="60">
+        <f>T76/T17</f>
+        <v>4.5587396635300852</v>
+      </c>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="B84" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.15">
+      <c r="B85" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3270,7 +4045,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="J42 J55" formula="1"/>
+    <ignoredError sqref="J42 J55 J8:J18 H42:H62" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>